<commit_message>
Update diccionario data gen
</commit_message>
<xml_diff>
--- a/Documentacion/Diccionario de datos.xlsx
+++ b/Documentacion/Diccionario de datos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="227">
   <si>
     <t>Nombre variable</t>
   </si>
@@ -267,9 +267,6 @@
     <t>Diccionario</t>
   </si>
   <si>
-    <t>int</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -670,6 +667,36 @@
   </si>
   <si>
     <t>Al escribir un caracter se actualiza la pagina</t>
+  </si>
+  <si>
+    <t>vec_size</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>new_data</t>
+  </si>
+  <si>
+    <t>vec</t>
+  </si>
+  <si>
+    <t>Par</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almacena vec y ts para agregarlos a las queues </t>
+  </si>
+  <si>
+    <t>Guarda los datos de las alarmas hasta almacenarlos en el queue</t>
+  </si>
+  <si>
+    <t>Guarda el time_stamp hasta almacenarlo en el queue</t>
+  </si>
+  <si>
+    <t>Recibe los datos desde el pipe y los distribuye a las distintas colas en base a los switches que esten o no activados</t>
+  </si>
+  <si>
+    <t>data_generation(thread)</t>
   </si>
 </sst>
 </file>
@@ -775,7 +802,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -803,18 +830,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -822,10 +840,23 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1133,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H155"/>
+  <dimension ref="A1:H152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,21 +1205,21 @@
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1269,7 +1300,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -1287,7 +1318,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -1305,7 +1336,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -1334,175 +1365,175 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="17" t="s">
         <v>61</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="13"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="13"/>
+        <v>209</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="17" t="s">
         <v>62</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="15" t="s">
+      <c r="F13" s="16"/>
+      <c r="G13" s="19" t="s">
         <v>35</v>
       </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="15"/>
+        <v>209</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="19"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="17" t="s">
         <v>63</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="19" t="s">
         <v>35</v>
       </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="15"/>
+        <v>209</v>
+      </c>
+      <c r="F16" s="16"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="17" t="s">
         <v>65</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="3"/>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G17" s="16" t="s">
         <v>35</v>
       </c>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="10"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
       <c r="D18" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
+        <v>209</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="17" t="s">
         <v>64</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="3"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12" t="s">
+      <c r="F19" s="16"/>
+      <c r="G19" s="16" t="s">
         <v>35</v>
       </c>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="10"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
+        <v>209</v>
+      </c>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1627,95 +1658,95 @@
       <c r="F26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="G26" s="12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="17" t="s">
         <v>70</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E27" s="2"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10" t="s">
+      <c r="F27" s="17"/>
+      <c r="G27" s="17" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
       <c r="D28" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
+        <v>208</v>
+      </c>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
     </row>
     <row r="29" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="17" t="s">
         <v>67</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
     </row>
     <row r="30" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
       <c r="D30" s="5" t="s">
         <v>47</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
+        <v>208</v>
+      </c>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
     </row>
     <row r="31" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16" t="s">
+      <c r="C31" s="13"/>
+      <c r="D31" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="17"/>
+      <c r="C32" s="21"/>
       <c r="D32" s="1" t="s">
         <v>13</v>
       </c>
@@ -1724,9 +1755,9 @@
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="17"/>
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="21"/>
       <c r="D33" s="1" t="s">
         <v>68</v>
       </c>
@@ -1736,14 +1767,14 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="8"/>
+      <c r="C34" s="14"/>
       <c r="D34" s="8" t="s">
         <v>13</v>
       </c>
@@ -1755,14 +1786,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>73</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="8"/>
+      <c r="C35" s="14"/>
       <c r="D35" s="8" t="s">
         <v>13</v>
       </c>
@@ -1774,14 +1805,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="8"/>
+      <c r="C36" s="14"/>
       <c r="D36" s="8" t="s">
         <v>13</v>
       </c>
@@ -1793,14 +1824,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>74</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="8"/>
+      <c r="C37" s="14"/>
       <c r="D37" s="8" t="s">
         <v>13</v>
       </c>
@@ -1812,14 +1843,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>75</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="8"/>
+      <c r="C38" s="14"/>
       <c r="D38" s="8" t="s">
         <v>13</v>
       </c>
@@ -1827,14 +1858,14 @@
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>76</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C39" s="8"/>
+      <c r="C39" s="14"/>
       <c r="D39" s="8" t="s">
         <v>13</v>
       </c>
@@ -1846,14 +1877,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>77</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" s="8"/>
+        <v>31</v>
+      </c>
+      <c r="C40" s="14"/>
       <c r="D40" s="8" t="s">
         <v>13</v>
       </c>
@@ -1865,14 +1896,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>78</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="8"/>
+        <v>31</v>
+      </c>
+      <c r="C41" s="14"/>
       <c r="D41" s="8" t="s">
         <v>13</v>
       </c>
@@ -1884,14 +1915,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
         <v>79</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C42" s="8"/>
+        <v>83</v>
+      </c>
+      <c r="C42" s="14"/>
       <c r="D42" s="8" t="s">
         <v>13</v>
       </c>
@@ -1903,14 +1934,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>80</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" s="8"/>
+        <v>84</v>
+      </c>
+      <c r="C43" s="14"/>
       <c r="D43" s="8" t="s">
         <v>13</v>
       </c>
@@ -1922,14 +1953,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
         <v>81</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" s="8"/>
+        <v>85</v>
+      </c>
+      <c r="C44" s="14"/>
       <c r="D44" s="8" t="s">
         <v>13</v>
       </c>
@@ -1941,116 +1972,116 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
     </row>
     <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
     </row>
     <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>35</v>
@@ -2059,258 +2090,258 @@
     </row>
     <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B51" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C51" s="8" t="s">
-        <v>145</v>
-      </c>
       <c r="D51" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
     </row>
     <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B52" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>147</v>
-      </c>
       <c r="D52" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
     </row>
     <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B53" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="C53" s="8" t="s">
-        <v>149</v>
-      </c>
       <c r="D53" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
     </row>
     <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>82</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
     </row>
     <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B55" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C55" s="8" t="s">
-        <v>152</v>
-      </c>
       <c r="D55" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
     </row>
     <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B56" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C56" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="C56" s="8" t="s">
-        <v>154</v>
-      </c>
       <c r="D56" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
     </row>
     <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B57" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C57" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="C57" s="8" t="s">
-        <v>208</v>
-      </c>
       <c r="D57" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
     </row>
     <row r="58" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
     </row>
     <row r="59" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B59" s="18"/>
+        <v>114</v>
+      </c>
+      <c r="B59" s="14"/>
       <c r="C59" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
     </row>
     <row r="60" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B61" s="8"/>
       <c r="C61" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F61" s="8"/>
       <c r="G61" s="8"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F64" s="8" t="s">
         <v>35</v>
@@ -2319,19 +2350,19 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F65" s="8" t="s">
         <v>35</v>
@@ -2340,76 +2371,76 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
     </row>
     <row r="67" spans="1:7" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B67" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="C67" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="C67" s="8" t="s">
-        <v>194</v>
-      </c>
       <c r="D67" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
     </row>
     <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
     </row>
     <row r="69" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F69" s="8"/>
       <c r="G69" s="8" t="s">
@@ -2418,270 +2449,306 @@
     </row>
     <row r="70" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B70" s="18"/>
+        <v>124</v>
+      </c>
+      <c r="B70" s="14"/>
       <c r="C70" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F70" s="8"/>
       <c r="G70" s="8"/>
     </row>
     <row r="71" spans="1:7" s="9" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B71" s="18"/>
+        <v>128</v>
+      </c>
+      <c r="B71" s="14"/>
       <c r="C71" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F71" s="8"/>
       <c r="G71" s="8"/>
     </row>
     <row r="72" spans="1:7" s="9" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B72" s="18"/>
+        <v>127</v>
+      </c>
+      <c r="B72" s="14"/>
       <c r="C72" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F72" s="8"/>
       <c r="G72" s="8"/>
     </row>
     <row r="73" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F73" s="8"/>
       <c r="G73" s="8"/>
     </row>
     <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F74" s="8"/>
       <c r="G74" s="8"/>
     </row>
     <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F75" s="8"/>
       <c r="G75" s="8"/>
     </row>
     <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B76" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C76" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="C76" s="8" t="s">
-        <v>201</v>
-      </c>
       <c r="D76" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F76" s="8"/>
       <c r="G76" s="8"/>
     </row>
     <row r="77" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B77" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C77" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="C77" s="8" t="s">
-        <v>204</v>
-      </c>
       <c r="D77" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F77" s="8"/>
       <c r="G77" s="8"/>
     </row>
     <row r="78" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B78" s="18"/>
+        <v>92</v>
+      </c>
+      <c r="B78" s="14"/>
       <c r="C78" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F78" s="8"/>
       <c r="G78" s="8"/>
     </row>
     <row r="79" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="B79" s="18"/>
+        <v>161</v>
+      </c>
+      <c r="B79" s="14"/>
       <c r="C79" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F79" s="8"/>
       <c r="G79" s="8"/>
     </row>
     <row r="80" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="B80" s="19" t="s">
-        <v>189</v>
+        <v>212</v>
+      </c>
+      <c r="B80" s="15" t="s">
+        <v>188</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F80" s="8"/>
       <c r="G80" s="8"/>
     </row>
     <row r="81" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F81" s="8"/>
       <c r="G81" s="8"/>
     </row>
     <row r="82" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="B82" s="18"/>
-      <c r="C82" s="18"/>
+        <v>211</v>
+      </c>
+      <c r="B82" s="14"/>
+      <c r="C82" s="14"/>
       <c r="D82" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F82" s="8"/>
       <c r="G82" s="8"/>
     </row>
-    <row r="83" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="8"/>
-      <c r="B83" s="8"/>
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8"/>
-      <c r="F83" s="8"/>
-      <c r="G83" s="8"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="8"/>
-      <c r="B84" s="8"/>
-      <c r="C84" s="8"/>
-      <c r="D84" s="8"/>
-      <c r="E84" s="8"/>
+    <row r="83" spans="1:7" s="11" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="D83" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="F83" s="10"/>
+      <c r="G83" s="10"/>
+    </row>
+    <row r="84" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B84" s="14"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E84" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="F84" s="8"/>
       <c r="G84" s="8"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="8"/>
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
-      <c r="D85" s="8"/>
-      <c r="E85" s="8"/>
+    <row r="85" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="D85" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E85" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="F85" s="8"/>
       <c r="G85" s="8"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="8"/>
-      <c r="B86" s="8"/>
-      <c r="C86" s="8"/>
-      <c r="D86" s="8"/>
-      <c r="E86" s="8"/>
+    <row r="86" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="D86" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E86" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="F86" s="8"/>
       <c r="G86" s="8"/>
     </row>
@@ -3279,45 +3346,21 @@
       <c r="F152" s="8"/>
       <c r="G152" s="8"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A153" s="8"/>
-      <c r="B153" s="8"/>
-      <c r="C153" s="8"/>
-      <c r="D153" s="8"/>
-      <c r="E153" s="8"/>
-      <c r="F153" s="8"/>
-      <c r="G153" s="8"/>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A154" s="8"/>
-      <c r="B154" s="8"/>
-      <c r="C154" s="8"/>
-      <c r="D154" s="8"/>
-      <c r="E154" s="8"/>
-      <c r="F154" s="8"/>
-      <c r="G154" s="8"/>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A155" s="8"/>
-      <c r="B155" s="8"/>
-      <c r="C155" s="8"/>
-      <c r="D155" s="8"/>
-      <c r="E155" s="8"/>
-      <c r="F155" s="8"/>
-      <c r="G155" s="8"/>
-    </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
@@ -3333,19 +3376,16 @@
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C17:C18"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G13:G14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E21" location="Sheet2!A1" display="delta_x()"/>
@@ -3358,10 +3398,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3418,22 +3458,22 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="17" t="s">
         <v>56</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="10"/>
+      <c r="F3" s="17"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -3441,14 +3481,14 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -3456,15 +3496,15 @@
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17" t="s">
         <v>57</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -3473,13 +3513,13 @@
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -3488,13 +3528,13 @@
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -3503,19 +3543,19 @@
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>87</v>
+      <c r="A8" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="17" t="s">
         <v>29</v>
       </c>
       <c r="F8" s="1"/>
@@ -3526,13 +3566,13 @@
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
+        <v>87</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -3541,13 +3581,13 @@
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -3556,13 +3596,13 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -3571,20 +3611,20 @@
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>91</v>
+      <c r="A12" s="17" t="s">
+        <v>90</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>96</v>
+      <c r="C12" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>95</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -3594,13 +3634,13 @@
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
+        <v>91</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -3609,15 +3649,15 @@
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+        <v>93</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -3626,15 +3666,15 @@
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="C15" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -3643,13 +3683,13 @@
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -3659,17 +3699,17 @@
     </row>
     <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -3680,17 +3720,17 @@
     </row>
     <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -3701,17 +3741,17 @@
     </row>
     <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -3721,20 +3761,20 @@
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>167</v>
+      <c r="A20" s="17" t="s">
+        <v>166</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D20" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>96</v>
+      <c r="D20" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>95</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -3744,15 +3784,15 @@
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
+        <v>178</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -3762,19 +3802,19 @@
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -3785,19 +3825,19 @@
     </row>
     <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="E23" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -3807,18 +3847,18 @@
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>170</v>
+      <c r="A24" s="17" t="s">
+        <v>169</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>96</v>
+        <v>183</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>95</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -3828,13 +3868,13 @@
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
+        <v>184</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
@@ -3844,19 +3884,19 @@
     </row>
     <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -3867,19 +3907,19 @@
     </row>
     <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -3889,11 +3929,19 @@
       <c r="K27" s="1"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="A28" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>47</v>
+      </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -3902,11 +3950,13 @@
       <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -3915,11 +3965,13 @@
       <c r="K29" s="1"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -3927,15 +3979,90 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="17"/>
+      <c r="B32" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="17"/>
+      <c r="B34" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="17"/>
+      <c r="B35" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="17"/>
+      <c r="B36" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="17"/>
+      <c r="B37" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="17"/>
+      <c r="B38" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+    </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="C24:C25"/>
+  <mergeCells count="26">
+    <mergeCell ref="A28:A38"/>
+    <mergeCell ref="C28:C38"/>
+    <mergeCell ref="D28:D38"/>
+    <mergeCell ref="E28:E38"/>
+    <mergeCell ref="E3:E7"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="D8:D11"/>
@@ -3945,12 +4072,13 @@
     <mergeCell ref="E12:E16"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E3:E7"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="C24:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Agregados datos y variables de alarmas (incompleto)
</commit_message>
<xml_diff>
--- a/Documentacion/Diccionario de datos.xlsx
+++ b/Documentacion/Diccionario de datos.xlsx
@@ -12,9 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="alarm_handler">Sheet2!$A$89</definedName>
+    <definedName name="alarmas_queue">Sheet2!$A$43</definedName>
     <definedName name="data_gen_parameters_source__DAS__time_stamp_DAS">Sheet2!$A$3</definedName>
     <definedName name="data_generation">Sheet2!$A$29</definedName>
     <definedName name="delta_x">Sheet2!$A$2</definedName>
+    <definedName name="encontrar_alarmas_live">Sheet2!$A$70</definedName>
     <definedName name="get_block">Sheet2!$A$21</definedName>
     <definedName name="new_folder_Date">Sheet2!$A$28</definedName>
     <definedName name="parse_markers">Sheet2!$A$27</definedName>
@@ -34,7 +37,7 @@
     <author>Dario</author>
   </authors>
   <commentList>
-    <comment ref="A63" authorId="0">
+    <comment ref="A64" authorId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="404">
   <si>
     <t>Nombre variable</t>
   </si>
@@ -954,6 +957,327 @@
   </si>
   <si>
     <t>"Alarmas ducto RA"</t>
+  </si>
+  <si>
+    <t>path_web</t>
+  </si>
+  <si>
+    <t>Path de la carpeta donde se encuentra los archivos de la web</t>
+  </si>
+  <si>
+    <t>'\\\Sscrdcrapl04\\Y-TEC\\WF\\web\\'</t>
+  </si>
+  <si>
+    <t>live_base</t>
+  </si>
+  <si>
+    <t>base_larga</t>
+  </si>
+  <si>
+    <t>bins</t>
+  </si>
+  <si>
+    <t>filename_base</t>
+  </si>
+  <si>
+    <t>alarm_queue</t>
+  </si>
+  <si>
+    <t>report_queue</t>
+  </si>
+  <si>
+    <t>now</t>
+  </si>
+  <si>
+    <t>logfile</t>
+  </si>
+  <si>
+    <t>dict_coords</t>
+  </si>
+  <si>
+    <t>dict_bins</t>
+  </si>
+  <si>
+    <t>window_count</t>
+  </si>
+  <si>
+    <t>bloque_inicial</t>
+  </si>
+  <si>
+    <t>data_report</t>
+  </si>
+  <si>
+    <t>matrix</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>fila_nueva</t>
+  </si>
+  <si>
+    <t>fila_zoneada</t>
+  </si>
+  <si>
+    <t>mean_base</t>
+  </si>
+  <si>
+    <t>std_base</t>
+  </si>
+  <si>
+    <t>u_m</t>
+  </si>
+  <si>
+    <t>u_c</t>
+  </si>
+  <si>
+    <t>timer_alarm_seg</t>
+  </si>
+  <si>
+    <t>timer_mail_ok_seg</t>
+  </si>
+  <si>
+    <t>timer_mail_ok</t>
+  </si>
+  <si>
+    <t>zonas_report</t>
+  </si>
+  <si>
+    <t>timer_alarm</t>
+  </si>
+  <si>
+    <t>max_pendiente</t>
+  </si>
+  <si>
+    <t>mail_send_ok</t>
+  </si>
+  <si>
+    <t>alarmas</t>
+  </si>
+  <si>
+    <t>ahora</t>
+  </si>
+  <si>
+    <t>txt_file</t>
+  </si>
+  <si>
+    <t>txt_mail</t>
+  </si>
+  <si>
+    <t>alarmas_cant</t>
+  </si>
+  <si>
+    <t>dict_img</t>
+  </si>
+  <si>
+    <t>kargs_mail</t>
+  </si>
+  <si>
+    <t>mail_tmp_file</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>cargar_base_larga</t>
+  </si>
+  <si>
+    <t>bins_inicio</t>
+  </si>
+  <si>
+    <t>bins_fin</t>
+  </si>
+  <si>
+    <t>parse_markers_coord</t>
+  </si>
+  <si>
+    <t>build_zone_dict</t>
+  </si>
+  <si>
+    <t>bin_dict</t>
+  </si>
+  <si>
+    <t>sub_zone_size</t>
+  </si>
+  <si>
+    <t>zone_dict</t>
+  </si>
+  <si>
+    <t>z_binning_vect</t>
+  </si>
+  <si>
+    <t>encontrar_alarmas_live</t>
+  </si>
+  <si>
+    <t>zona</t>
+  </si>
+  <si>
+    <t>window</t>
+  </si>
+  <si>
+    <t>funciones_alarmas.py</t>
+  </si>
+  <si>
+    <t>binned_matrix.mean(0)</t>
+  </si>
+  <si>
+    <t>alarma_fila_nueva</t>
+  </si>
+  <si>
+    <t>np.max(matriz_umbrales,axis=0)</t>
+  </si>
+  <si>
+    <t>reporte</t>
+  </si>
+  <si>
+    <t>umbrales_matriz</t>
+  </si>
+  <si>
+    <t>umbrales_cuenta</t>
+  </si>
+  <si>
+    <t>primera_fila_alarma</t>
+  </si>
+  <si>
+    <t>Almacena el tiempo actual</t>
+  </si>
+  <si>
+    <t>datetime.datetime.now().strftime</t>
+  </si>
+  <si>
+    <t>Buffer para la imagen</t>
+  </si>
+  <si>
+    <t>glob.glob</t>
+  </si>
+  <si>
+    <t>Almacena el/los paths que coincidan con el agurmento(en este caso, 'C:/test base larga/1_madrugada/STD/0*.std') para luego levantar los archivos que se encuentren en ese lugar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>path_alarmas_log</t>
+  </si>
+  <si>
+    <t>'alarmas_log/'</t>
+  </si>
+  <si>
+    <t>Almacena el indice al archivo para almacenar el log</t>
+  </si>
+  <si>
+    <t>Almacena un diccionario con los nombres de las zonas y las coordenadas</t>
+  </si>
+  <si>
+    <t>Almacena un diccionario con los nombres de las zonas y los bines</t>
+  </si>
+  <si>
+    <t>Almacena una nueva fila de  alarm_queue</t>
+  </si>
+  <si>
+    <t>Almacena las nuevas filas de alarm_queue para luego procesarlas</t>
+  </si>
+  <si>
+    <t>Almacena un nuevo ts de alarm_queue</t>
+  </si>
+  <si>
+    <t>Almacena la nueva fila zoneada</t>
+  </si>
+  <si>
+    <t>Almacena los valores medios de la base. En el caso de que no encuentre el archivo donde los datos estan almacenados lo crea con los nuevos datos que le van llegando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almacena los valores medios del std para </t>
+  </si>
+  <si>
+    <t>Checkea si se quiere tomar la base en vivo o si se tiene una almacenada</t>
+  </si>
+  <si>
+    <t>np.zeros((rows_plot, bins))</t>
+  </si>
+  <si>
+    <t>alarm_queue.popleft()</t>
+  </si>
+  <si>
+    <t>encontrar_alarmas_live(...)</t>
+  </si>
+  <si>
+    <t>60*4</t>
+  </si>
+  <si>
+    <t>time.time()</t>
+  </si>
+  <si>
+    <t>60*60*4</t>
+  </si>
+  <si>
+    <t>np.array([])</t>
+  </si>
+  <si>
+    <t>tt</t>
+  </si>
+  <si>
+    <t>last_mail</t>
+  </si>
+  <si>
+    <t>silence_dict</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>th_launch(zone_watcher, [silence_dict])</t>
+  </si>
+  <si>
+    <t>alarma_fila_nueva(...)</t>
+  </si>
+  <si>
+    <t>Ve cuantos std hay en la cola para procesar</t>
+  </si>
+  <si>
+    <t>alarm_handler</t>
+  </si>
+  <si>
+    <t>Matriz con unos donde supera el umbral de la zona y con 0 donde no</t>
+  </si>
+  <si>
+    <t>Arreglo con los resultados de sumar cada valor de una columna</t>
+  </si>
+  <si>
+    <t>Lanza el thread que silencia alarmas</t>
+  </si>
+  <si>
+    <t>timer_alarm_ok_seg</t>
+  </si>
+  <si>
+    <t>reporte(...)</t>
+  </si>
+  <si>
+    <t>Guarda la hora del mail</t>
+  </si>
+  <si>
+    <t>Guarda la hora de la alarma</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>zone_watcher</t>
+  </si>
+  <si>
+    <t>check_freq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checkea mediante los deadlines de las zonas silenciadas para activarlas cuando termine el tiempo indicado </t>
+  </si>
+  <si>
+    <t>Calcula los umbrales_matriz(u_m) y los umbrales_cuenta(u_c) los cuales luego van a ser utilizados para reconocer alarmas</t>
+  </si>
+  <si>
+    <t>Actualiza los u_m y u_c y devuelve un arreglo con los valores maximos de cada zona</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1423,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1172,10 +1496,64 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1196,10 +1574,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1507,10 +1882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H148"/>
+  <dimension ref="A1:H151"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="G96" sqref="G96"/>
+    <sheetView topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="H112" sqref="H112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1820,7 +2195,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>52</v>
       </c>
@@ -1842,11 +2217,11 @@
         <v>247</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="20" t="s">
         <v>260</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1864,7 +2239,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1982,74 +2357,74 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="48" t="s">
         <v>65</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E22" s="2"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30" t="s">
+      <c r="F22" s="48"/>
+      <c r="G22" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="H22" s="28" t="s">
+      <c r="H22" s="47" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
+      <c r="A23" s="48"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
       <c r="D23" s="4" t="s">
         <v>45</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="28"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="47"/>
     </row>
     <row r="24" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="48" t="s">
         <v>62</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="28" t="s">
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="47" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
+      <c r="A25" s="48"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
       <c r="D25" s="4" t="s">
         <v>45</v>
       </c>
       <c r="E25" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="28"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="47"/>
     </row>
     <row r="26" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
@@ -2059,7 +2434,7 @@
         <v>43</v>
       </c>
       <c r="C26" s="12"/>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E26" s="12"/>
@@ -2070,27 +2445,27 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="35"/>
+      <c r="C27" s="53"/>
       <c r="D27" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="28" t="s">
+      <c r="H27" s="47" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="30"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="35"/>
+      <c r="A28" s="48"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="53"/>
       <c r="D28" s="4" t="s">
         <v>63</v>
       </c>
@@ -2099,7 +2474,7 @@
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="28"/>
+      <c r="H28" s="47"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
@@ -2361,37 +2736,37 @@
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D41" s="4" t="s">
+    <row r="41" spans="1:8" s="20" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="D41" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="E41" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="17" t="s">
-        <v>116</v>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="G41" s="28"/>
+      <c r="H41" s="35" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>133</v>
+        <v>199</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>90</v>
@@ -2399,23 +2774,21 @@
       <c r="E42" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F42" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="19">
-        <v>100</v>
+      <c r="H42" s="17" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>132</v>
+        <v>30</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>90</v>
@@ -2423,21 +2796,23 @@
       <c r="E43" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F43" s="7"/>
+      <c r="F43" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="G43" s="7"/>
-      <c r="H43" s="19" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H43" s="19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>90</v>
@@ -2447,19 +2822,19 @@
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
-      <c r="H44" s="27" t="s">
-        <v>270</v>
+      <c r="H44" s="19" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>90</v>
@@ -2475,13 +2850,13 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>30</v>
+        <v>131</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>90</v>
@@ -2489,23 +2864,21 @@
       <c r="E46" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F46" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="F46" s="7"/>
       <c r="G46" s="7"/>
-      <c r="H46" s="19">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H46" s="27" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>138</v>
+        <v>30</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>90</v>
@@ -2513,21 +2886,23 @@
       <c r="E47" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F47" s="7"/>
+      <c r="F47" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="G47" s="7"/>
-      <c r="H47" s="27" t="s">
-        <v>269</v>
+      <c r="H47" s="19">
+        <v>400</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>90</v>
@@ -2538,18 +2913,18 @@
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
       <c r="H48" s="27" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>90</v>
@@ -2560,18 +2935,18 @@
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
       <c r="H49" s="27" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>77</v>
+        <v>142</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>90</v>
@@ -2582,18 +2957,18 @@
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
       <c r="H50" s="27" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>145</v>
+        <v>77</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>254</v>
+        <v>144</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>90</v>
@@ -2604,18 +2979,18 @@
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
       <c r="H51" s="27" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>147</v>
+        <v>254</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>90</v>
@@ -2626,18 +3001,18 @@
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
       <c r="H52" s="27" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>196</v>
+        <v>146</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>197</v>
+        <v>147</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>90</v>
@@ -2647,17 +3022,19 @@
       </c>
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
-      <c r="H53" s="19"/>
-    </row>
-    <row r="54" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H53" s="27" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>90</v>
@@ -2669,13 +3046,15 @@
       <c r="G54" s="7"/>
       <c r="H54" s="19"/>
     </row>
-    <row r="55" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B55" s="13"/>
+        <v>94</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>195</v>
+      </c>
       <c r="C55" s="7" t="s">
-        <v>149</v>
+        <v>194</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>90</v>
@@ -2685,19 +3064,15 @@
       </c>
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
-      <c r="H55" s="27" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H55" s="19"/>
+    </row>
+    <row r="56" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>152</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="B56" s="13"/>
       <c r="C56" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>90</v>
@@ -2708,16 +3083,18 @@
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
       <c r="H56" s="27" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57" s="7" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B57" s="7"/>
       <c r="C57" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>90</v>
@@ -2728,18 +3105,16 @@
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
       <c r="H57" s="27" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>151</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B58" s="7"/>
       <c r="C58" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>90</v>
@@ -2750,15 +3125,19 @@
       <c r="F58" s="7"/>
       <c r="G58" s="7"/>
       <c r="H58" s="27" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B59" s="7" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B59" s="18"/>
-      <c r="C59" s="18"/>
+      <c r="C59" s="7" t="s">
+        <v>150</v>
+      </c>
       <c r="D59" s="4" t="s">
         <v>90</v>
       </c>
@@ -2768,42 +3147,36 @@
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
       <c r="H59" s="27" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>153</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B60" s="18"/>
+      <c r="C60" s="18"/>
       <c r="D60" s="4" t="s">
         <v>90</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F60" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="F60" s="7"/>
       <c r="G60" s="7"/>
-      <c r="H60" s="19">
-        <v>3400</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H60" s="27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>90</v>
@@ -2816,18 +3189,18 @@
       </c>
       <c r="G61" s="7"/>
       <c r="H61" s="19">
-        <v>10300</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="17" t="s">
-        <v>276</v>
-      </c>
-      <c r="B62" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C62" s="17" t="s">
-        <v>277</v>
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>90</v>
@@ -2835,21 +3208,23 @@
       <c r="E62" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F62" s="17"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="19" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>184</v>
+      <c r="F62" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G62" s="7"/>
+      <c r="H62" s="19">
+        <v>10300</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>277</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>90</v>
@@ -2857,19 +3232,21 @@
       <c r="E63" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="19"/>
-    </row>
-    <row r="64" spans="1:8" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="19" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>185</v>
+        <v>116</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>186</v>
+        <v>30</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>90</v>
@@ -2879,19 +3256,17 @@
       </c>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
-      <c r="H64" s="27" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H64" s="19"/>
+    </row>
+    <row r="65" spans="1:8" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>117</v>
+        <v>185</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>186</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>90</v>
@@ -2905,15 +3280,15 @@
         <v>280</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>30</v>
+        <v>186</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>90</v>
@@ -2922,20 +3297,20 @@
         <v>85</v>
       </c>
       <c r="F66" s="7"/>
-      <c r="G66" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H66" s="19" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G66" s="7"/>
+      <c r="H66" s="27" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="B67" s="13"/>
+        <v>118</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="C67" s="7" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>90</v>
@@ -2944,18 +3319,20 @@
         <v>85</v>
       </c>
       <c r="F67" s="7"/>
-      <c r="G67" s="7"/>
+      <c r="G67" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="H67" s="19" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" s="8" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B68" s="13"/>
       <c r="C68" s="7" t="s">
-        <v>158</v>
+        <v>205</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>90</v>
@@ -2965,17 +3342,17 @@
       </c>
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
-      <c r="H68" s="27" t="s">
-        <v>160</v>
+      <c r="H68" s="19" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="8" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B69" s="13"/>
       <c r="C69" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>90</v>
@@ -2989,15 +3366,13 @@
         <v>160</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" s="8" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>186</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="B70" s="13"/>
       <c r="C70" s="7" t="s">
-        <v>190</v>
+        <v>159</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>90</v>
@@ -3008,18 +3383,18 @@
       <c r="F70" s="7"/>
       <c r="G70" s="7"/>
       <c r="H70" s="27" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>186</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>90</v>
@@ -3033,15 +3408,15 @@
         <v>280</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>90</v>
@@ -3052,16 +3427,18 @@
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
       <c r="H72" s="27" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B73" s="13"/>
+        <v>95</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>182</v>
+      </c>
       <c r="C73" s="7" t="s">
-        <v>156</v>
+        <v>192</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>90</v>
@@ -3072,16 +3449,16 @@
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
       <c r="H73" s="27" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
-        <v>155</v>
+        <v>87</v>
       </c>
       <c r="B74" s="13"/>
       <c r="C74" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>90</v>
@@ -3092,18 +3469,16 @@
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
       <c r="H74" s="27" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="B75" s="14" t="s">
-        <v>182</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="B75" s="13"/>
       <c r="C75" s="7" t="s">
-        <v>203</v>
+        <v>157</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>90</v>
@@ -3113,19 +3488,19 @@
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
-      <c r="H75" s="19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H75" s="27" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>193</v>
+        <v>201</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>182</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>90</v>
@@ -3135,16 +3510,20 @@
       </c>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
-      <c r="H76" s="27" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H76" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="B77" s="13"/>
-      <c r="C77" s="13"/>
+        <v>202</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>204</v>
+      </c>
       <c r="D77" s="4" t="s">
         <v>90</v>
       </c>
@@ -3153,72 +3532,68 @@
       </c>
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
-      <c r="H77" s="19" t="s">
+      <c r="H77" s="27" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B78" s="13"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="19" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="78" spans="1:8" s="10" customFormat="1" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="30" t="s">
+    <row r="79" spans="1:8" s="10" customFormat="1" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="48" t="s">
         <v>209</v>
       </c>
-      <c r="B78" s="31" t="s">
+      <c r="B79" s="49" t="s">
         <v>173</v>
       </c>
-      <c r="C78" s="31" t="s">
+      <c r="C79" s="49" t="s">
         <v>212</v>
       </c>
-      <c r="D78" s="33" t="s">
+      <c r="D79" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="E78" s="33" t="s">
+      <c r="E79" s="51" t="s">
         <v>198</v>
       </c>
-      <c r="F78" s="34"/>
-      <c r="G78" s="30"/>
-      <c r="H78" s="19" t="s">
+      <c r="F79" s="52"/>
+      <c r="G79" s="48"/>
+      <c r="H79" s="19" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="79" spans="1:8" s="20" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="30"/>
-      <c r="B79" s="32"/>
-      <c r="C79" s="32"/>
-      <c r="D79" s="33"/>
-      <c r="E79" s="33"/>
-      <c r="F79" s="34"/>
-      <c r="G79" s="30"/>
-      <c r="H79" s="27" t="s">
+    <row r="80" spans="1:8" s="20" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="48"/>
+      <c r="B80" s="50"/>
+      <c r="C80" s="50"/>
+      <c r="D80" s="51"/>
+      <c r="E80" s="51"/>
+      <c r="F80" s="52"/>
+      <c r="G80" s="48"/>
+      <c r="H80" s="27" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="7" t="s">
+    <row r="81" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="B80" s="13"/>
-      <c r="C80" s="13"/>
-      <c r="D80" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="F80" s="7"/>
-      <c r="G80" s="7"/>
-      <c r="H80" s="19" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>213</v>
-      </c>
+      <c r="B81" s="13"/>
+      <c r="C81" s="13"/>
       <c r="D81" s="4" t="s">
         <v>45</v>
       </c>
@@ -3227,19 +3602,19 @@
       </c>
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
-      <c r="H81" s="27" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H81" s="19" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>208</v>
+        <v>172</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>210</v>
+        <v>79</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>45</v>
@@ -3249,41 +3624,41 @@
       </c>
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
-      <c r="H82" s="19" t="s">
-        <v>288</v>
+      <c r="H82" s="27" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>227</v>
+        <v>45</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>228</v>
+        <v>198</v>
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
-      <c r="H83" s="27" t="s">
+      <c r="H83" s="19" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B84" s="7" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>193</v>
-      </c>
       <c r="C84" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>227</v>
@@ -3293,17 +3668,19 @@
       </c>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
-      <c r="H84" s="37" t="s">
-        <v>296</v>
+      <c r="H84" s="27" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="B85" s="7"/>
+        <v>216</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="C85" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>227</v>
@@ -3313,19 +3690,17 @@
       </c>
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
-      <c r="H85" s="27" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H85" s="30" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>232</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="B86" s="7"/>
       <c r="C86" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>227</v>
@@ -3336,18 +3711,18 @@
       <c r="F86" s="7"/>
       <c r="G86" s="7"/>
       <c r="H86" s="27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>227</v>
@@ -3358,18 +3733,18 @@
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
       <c r="H87" s="27" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>79</v>
+        <v>235</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>227</v>
@@ -3379,19 +3754,19 @@
       </c>
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
-      <c r="H88" s="19" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H88" s="27" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>237</v>
+        <v>79</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>227</v>
@@ -3401,19 +3776,19 @@
       </c>
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
-      <c r="H89" s="27" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="H89" s="19" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>79</v>
+        <v>237</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>227</v>
@@ -3423,19 +3798,19 @@
       </c>
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
-      <c r="H90" s="19" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H90" s="27" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B91" s="7" t="s">
         <v>79</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>227</v>
@@ -3449,15 +3824,15 @@
         <v>293</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>237</v>
+        <v>79</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>227</v>
@@ -3467,18 +3842,20 @@
       </c>
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
-      <c r="H92" s="27" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H92" s="19" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B93" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="C93" s="16"/>
+      <c r="C93" s="7" t="s">
+        <v>240</v>
+      </c>
       <c r="D93" s="4" t="s">
         <v>227</v>
       </c>
@@ -3491,14 +3868,14 @@
         <v>292</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="B94" s="16"/>
-      <c r="C94" s="7" t="s">
-        <v>243</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C94" s="16"/>
       <c r="D94" s="4" t="s">
         <v>227</v>
       </c>
@@ -3508,339 +3885,722 @@
       <c r="F94" s="7"/>
       <c r="G94" s="7"/>
       <c r="H94" s="27" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="7"/>
-      <c r="B95" s="7"/>
-      <c r="C95" s="7"/>
-      <c r="D95" s="7"/>
-      <c r="E95" s="7"/>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B95" s="16"/>
+      <c r="C95" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>228</v>
+      </c>
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="7"/>
-      <c r="B96" s="7"/>
-      <c r="C96" s="7"/>
-      <c r="D96" s="7"/>
-      <c r="E96" s="7"/>
+      <c r="H95" s="27" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="D96" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E96" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="7"/>
-      <c r="B97" s="7"/>
-      <c r="C97" s="7"/>
-      <c r="D97" s="7"/>
-      <c r="E97" s="7"/>
+      <c r="H96" s="34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A97" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="D97" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E97" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F97" s="7"/>
       <c r="G97" s="7"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="7"/>
-      <c r="B98" s="7"/>
-      <c r="C98" s="7"/>
-      <c r="D98" s="7"/>
-      <c r="E98" s="7"/>
+      <c r="H97" s="42" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="D98" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E98" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F98" s="7"/>
       <c r="G98" s="7"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="7"/>
-      <c r="B99" s="7"/>
-      <c r="C99" s="7"/>
-      <c r="D99" s="7"/>
-      <c r="E99" s="7"/>
+      <c r="H98" s="38" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="D99" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E99" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F99" s="7"/>
       <c r="G99" s="7"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="7"/>
-      <c r="B100" s="7"/>
-      <c r="C100" s="7"/>
-      <c r="D100" s="7"/>
-      <c r="E100" s="7"/>
+      <c r="H99" s="43" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="D100" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E100" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="7"/>
-      <c r="B101" s="7"/>
-      <c r="C101" s="7"/>
-      <c r="D101" s="7"/>
-      <c r="E101" s="7"/>
+    <row r="101" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A101" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="D101" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E101" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F101" s="7"/>
       <c r="G101" s="7"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="7"/>
-      <c r="B102" s="7"/>
-      <c r="C102" s="7"/>
-      <c r="D102" s="7"/>
-      <c r="E102" s="7"/>
+    <row r="102" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="D102" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E102" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F102" s="7"/>
       <c r="G102" s="7"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="7"/>
-      <c r="B103" s="7"/>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>260</v>
+      </c>
       <c r="C103" s="7"/>
-      <c r="D103" s="7"/>
-      <c r="E103" s="7"/>
+      <c r="D103" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E103" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F103" s="7"/>
       <c r="G103" s="7"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="7"/>
-      <c r="B104" s="7"/>
-      <c r="C104" s="7"/>
-      <c r="D104" s="7"/>
-      <c r="E104" s="7"/>
+    <row r="104" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="D104" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E104" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F104" s="7"/>
       <c r="G104" s="7"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="7"/>
-      <c r="B105" s="7"/>
-      <c r="C105" s="7"/>
-      <c r="D105" s="7"/>
-      <c r="E105" s="7"/>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="D105" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E105" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F105" s="7"/>
       <c r="G105" s="7"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="7"/>
+      <c r="H105" s="39" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106" s="7" t="s">
+        <v>315</v>
+      </c>
       <c r="B106" s="7"/>
-      <c r="C106" s="7"/>
-      <c r="D106" s="7"/>
-      <c r="E106" s="7"/>
+      <c r="C106" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="D106" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E106" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F106" s="7"/>
       <c r="G106" s="7"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="7"/>
+      <c r="H106" s="39" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="7" t="s">
+        <v>172</v>
+      </c>
       <c r="B107" s="7"/>
-      <c r="C107" s="7"/>
-      <c r="D107" s="7"/>
-      <c r="E107" s="7"/>
+      <c r="C107" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="D107" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E107" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F107" s="7"/>
       <c r="G107" s="7"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="7"/>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="7" t="s">
+        <v>316</v>
+      </c>
       <c r="B108" s="7"/>
-      <c r="C108" s="7"/>
-      <c r="D108" s="7"/>
-      <c r="E108" s="7"/>
+      <c r="C108" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="D108" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E108" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F108" s="7"/>
       <c r="G108" s="7"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="7"/>
+    <row r="109" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A109" s="7" t="s">
+        <v>317</v>
+      </c>
       <c r="B109" s="7"/>
-      <c r="C109" s="7"/>
-      <c r="D109" s="7"/>
-      <c r="E109" s="7"/>
+      <c r="C109" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="D109" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E109" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F109" s="7"/>
       <c r="G109" s="7"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="7"/>
+    <row r="110" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="7" t="s">
+        <v>318</v>
+      </c>
       <c r="B110" s="7"/>
-      <c r="C110" s="7"/>
-      <c r="D110" s="7"/>
-      <c r="E110" s="7"/>
+      <c r="C110" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="D110" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E110" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F110" s="7"/>
       <c r="G110" s="7"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="7"/>
+    <row r="111" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A111" s="7" t="s">
+        <v>319</v>
+      </c>
       <c r="B111" s="7"/>
-      <c r="C111" s="7"/>
-      <c r="D111" s="7"/>
-      <c r="E111" s="7"/>
+      <c r="C111" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="D111" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E111" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F111" s="7"/>
       <c r="G111" s="7"/>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="7"/>
+      <c r="H111" s="45" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="7" t="s">
+        <v>320</v>
+      </c>
       <c r="B112" s="7"/>
-      <c r="C112" s="7"/>
-      <c r="D112" s="7"/>
-      <c r="E112" s="7"/>
+      <c r="C112" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="D112" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E112" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F112" s="7"/>
       <c r="G112" s="7"/>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="7"/>
-      <c r="B113" s="7"/>
+      <c r="H112" s="45" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>260</v>
+      </c>
       <c r="C113" s="7"/>
-      <c r="D113" s="7"/>
-      <c r="E113" s="7"/>
-      <c r="F113" s="7"/>
+      <c r="D113" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E113" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="F113" s="7" t="s">
+        <v>397</v>
+      </c>
       <c r="G113" s="7"/>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="7"/>
-      <c r="B114" s="7"/>
-      <c r="C114" s="7"/>
-      <c r="D114" s="7"/>
-      <c r="E114" s="7"/>
+      <c r="H113" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="D114" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E114" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F114" s="7"/>
       <c r="G114" s="7"/>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="7"/>
-      <c r="B115" s="7"/>
+      <c r="H114" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>260</v>
+      </c>
       <c r="C115" s="7"/>
-      <c r="D115" s="7"/>
-      <c r="E115" s="7"/>
-      <c r="F115" s="7"/>
+      <c r="D115" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E115" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="F115" s="7" t="s">
+        <v>398</v>
+      </c>
       <c r="G115" s="7"/>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="7"/>
-      <c r="B116" s="7"/>
-      <c r="C116" s="7"/>
-      <c r="D116" s="7"/>
-      <c r="E116" s="7"/>
+      <c r="H115" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="D116" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E116" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F116" s="7"/>
       <c r="G116" s="7"/>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="7"/>
-      <c r="B117" s="7"/>
+      <c r="H116" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="C117" s="7"/>
-      <c r="D117" s="7"/>
-      <c r="E117" s="7"/>
+      <c r="D117" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E117" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F117" s="7"/>
       <c r="G117" s="7"/>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="7"/>
-      <c r="B118" s="7"/>
-      <c r="C118" s="7"/>
-      <c r="D118" s="7"/>
-      <c r="E118" s="7"/>
+      <c r="H117" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="D118" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E118" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F118" s="7"/>
       <c r="G118" s="7"/>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="7"/>
-      <c r="B119" s="7"/>
+      <c r="H118" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>196</v>
+      </c>
       <c r="C119" s="7"/>
-      <c r="D119" s="7"/>
-      <c r="E119" s="7"/>
+      <c r="D119" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E119" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F119" s="7"/>
       <c r="G119" s="7"/>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="7"/>
-      <c r="B120" s="7"/>
-      <c r="C120" s="7"/>
-      <c r="D120" s="7"/>
-      <c r="E120" s="7"/>
-      <c r="F120" s="7"/>
-      <c r="G120" s="7"/>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="7"/>
-      <c r="B121" s="7"/>
-      <c r="C121" s="7"/>
-      <c r="D121" s="7"/>
-      <c r="E121" s="7"/>
-      <c r="F121" s="7"/>
-      <c r="G121" s="7"/>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="7"/>
-      <c r="B122" s="7"/>
-      <c r="C122" s="7"/>
-      <c r="D122" s="7"/>
-      <c r="E122" s="7"/>
-      <c r="F122" s="7"/>
-      <c r="G122" s="7"/>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A123" s="7"/>
+      <c r="H119" s="41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="39" t="s">
+        <v>383</v>
+      </c>
+      <c r="B120" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C120" s="39"/>
+      <c r="D120" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E120" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="F120" s="39"/>
+      <c r="G120" s="39"/>
+      <c r="H120" s="20" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="39" t="s">
+        <v>384</v>
+      </c>
+      <c r="B121" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C121" s="39"/>
+      <c r="D121" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E121" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="F121" s="39"/>
+      <c r="G121" s="39"/>
+      <c r="H121" s="20" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="39" t="s">
+        <v>382</v>
+      </c>
+      <c r="B122" s="39"/>
+      <c r="C122" s="39" t="s">
+        <v>392</v>
+      </c>
+      <c r="D122" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E122" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="F122" s="39"/>
+      <c r="G122" s="39"/>
+      <c r="H122" s="20" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="7" t="s">
+        <v>328</v>
+      </c>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
-      <c r="D123" s="7"/>
-      <c r="E123" s="7"/>
+      <c r="D123" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E123" s="33" t="s">
+        <v>64</v>
+      </c>
       <c r="F123" s="7"/>
       <c r="G123" s="7"/>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" s="7"/>
+      <c r="H123" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="7" t="s">
+        <v>329</v>
+      </c>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
-      <c r="D124" s="7"/>
-      <c r="E124" s="7"/>
+      <c r="D124" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E124" s="40" t="s">
+        <v>389</v>
+      </c>
       <c r="F124" s="7"/>
       <c r="G124" s="7"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" s="7"/>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="7" t="s">
+        <v>330</v>
+      </c>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>
-      <c r="D125" s="7"/>
-      <c r="E125" s="7"/>
+      <c r="D125" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E125" s="40" t="s">
+        <v>389</v>
+      </c>
       <c r="F125" s="7"/>
       <c r="G125" s="7"/>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A126" s="7"/>
+      <c r="H125" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="7" t="s">
+        <v>331</v>
+      </c>
       <c r="B126" s="7"/>
       <c r="C126" s="7"/>
-      <c r="D126" s="7"/>
-      <c r="E126" s="7"/>
+      <c r="D126" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E126" s="40" t="s">
+        <v>389</v>
+      </c>
       <c r="F126" s="7"/>
       <c r="G126" s="7"/>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" s="7"/>
+      <c r="H126" s="20" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" s="7" t="s">
+        <v>332</v>
+      </c>
       <c r="B127" s="7"/>
       <c r="C127" s="7"/>
-      <c r="D127" s="7"/>
-      <c r="E127" s="7"/>
+      <c r="D127" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E127" s="40" t="s">
+        <v>389</v>
+      </c>
       <c r="F127" s="7"/>
       <c r="G127" s="7"/>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A128" s="7"/>
-      <c r="B128" s="7"/>
+      <c r="H127" s="20" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="C128" s="7"/>
-      <c r="D128" s="7"/>
-      <c r="E128" s="7"/>
+      <c r="D128" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E128" s="40" t="s">
+        <v>389</v>
+      </c>
       <c r="F128" s="7"/>
       <c r="G128" s="7"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A129" s="7"/>
-      <c r="B129" s="7"/>
+      <c r="A129" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="C129" s="7"/>
-      <c r="D129" s="7"/>
-      <c r="E129" s="7"/>
+      <c r="D129" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E129" s="40" t="s">
+        <v>389</v>
+      </c>
       <c r="F129" s="7"/>
       <c r="G129" s="7"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="7"/>
-      <c r="B130" s="7"/>
+      <c r="A130" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>336</v>
+      </c>
       <c r="C130" s="7"/>
-      <c r="D130" s="7"/>
-      <c r="E130" s="7"/>
+      <c r="D130" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E130" s="40" t="s">
+        <v>389</v>
+      </c>
       <c r="F130" s="7"/>
       <c r="G130" s="7"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A131" s="7"/>
-      <c r="B131" s="7"/>
+      <c r="A131" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>260</v>
+      </c>
       <c r="C131" s="7"/>
-      <c r="D131" s="7"/>
-      <c r="E131" s="7"/>
+      <c r="D131" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E131" s="40" t="s">
+        <v>64</v>
+      </c>
       <c r="F131" s="7"/>
       <c r="G131" s="7"/>
     </row>
@@ -3849,7 +4609,7 @@
       <c r="B132" s="7"/>
       <c r="C132" s="7"/>
       <c r="D132" s="7"/>
-      <c r="E132" s="7"/>
+      <c r="E132" s="33"/>
       <c r="F132" s="7"/>
       <c r="G132" s="7"/>
     </row>
@@ -3996,6 +4756,33 @@
       <c r="E148" s="7"/>
       <c r="F148" s="7"/>
       <c r="G148" s="7"/>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" s="7"/>
+      <c r="B149" s="7"/>
+      <c r="C149" s="7"/>
+      <c r="D149" s="7"/>
+      <c r="E149" s="7"/>
+      <c r="F149" s="7"/>
+      <c r="G149" s="7"/>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" s="7"/>
+      <c r="B150" s="7"/>
+      <c r="C150" s="7"/>
+      <c r="D150" s="7"/>
+      <c r="E150" s="7"/>
+      <c r="F150" s="7"/>
+      <c r="G150" s="7"/>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" s="7"/>
+      <c r="B151" s="7"/>
+      <c r="C151" s="7"/>
+      <c r="D151" s="7"/>
+      <c r="E151" s="7"/>
+      <c r="F151" s="7"/>
+      <c r="G151" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="23">
@@ -4009,13 +4796,13 @@
     <mergeCell ref="H22:H23"/>
     <mergeCell ref="H24:H25"/>
     <mergeCell ref="H27:H28"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="E78:E79"/>
-    <mergeCell ref="F78:F79"/>
-    <mergeCell ref="G78:G79"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="C27:C28"/>
@@ -4030,11 +4817,11 @@
     <hyperlink ref="E20" location="delta_x" display="delta_x"/>
     <hyperlink ref="E23" location="data_generation" display="data_generation"/>
     <hyperlink ref="E25" location="data_generation" display="data_generation"/>
-    <hyperlink ref="E41" location="plot_setup" display="plot_setup"/>
-    <hyperlink ref="E78" location="data_generation" display="data_generation"/>
-    <hyperlink ref="E80:E82" location="data_generation" display="data_generation"/>
-    <hyperlink ref="E83" location="server_opc" display="server_opc"/>
-    <hyperlink ref="E84:E94" location="server_opc" display="server_opc"/>
+    <hyperlink ref="E42" location="plot_setup" display="plot_setup"/>
+    <hyperlink ref="E79" location="data_generation" display="data_generation"/>
+    <hyperlink ref="E81:E83" location="data_generation" display="data_generation"/>
+    <hyperlink ref="E84" location="server_opc" display="server_opc"/>
+    <hyperlink ref="E85:E95" location="server_opc" display="server_opc"/>
     <hyperlink ref="D3" r:id="rId1"/>
     <hyperlink ref="D4:D11" r:id="rId2" display="test_marco1_m.py"/>
     <hyperlink ref="D12" r:id="rId3"/>
@@ -4049,9 +4836,9 @@
     <hyperlink ref="D29" r:id="rId12"/>
     <hyperlink ref="D30" r:id="rId13"/>
     <hyperlink ref="D16:D20" r:id="rId14" display="func_aux_main.py"/>
-    <hyperlink ref="D41" r:id="rId15"/>
-    <hyperlink ref="D77" r:id="rId16"/>
-    <hyperlink ref="D83:D94" r:id="rId17" display="func_opc.py"/>
+    <hyperlink ref="D42" r:id="rId15"/>
+    <hyperlink ref="D78" r:id="rId16"/>
+    <hyperlink ref="D84:D95" r:id="rId17" display="func_opc.py"/>
     <hyperlink ref="D25" r:id="rId18"/>
     <hyperlink ref="D23" r:id="rId19"/>
     <hyperlink ref="D28" r:id="rId20"/>
@@ -4062,56 +4849,62 @@
     <hyperlink ref="H14" location="data_gen_parameters_source__DAS__time_stamp_DAS" display="data_gen_parameters()"/>
     <hyperlink ref="H15" location="data_gen_parameters_source__DAS__time_stamp_DAS" display="data_gen_parameters()"/>
     <hyperlink ref="H40" location="th_launch" display="th_launch"/>
-    <hyperlink ref="H44" r:id="rId21" display="plt.subplots(figsize=(20, 10))"/>
-    <hyperlink ref="H45" r:id="rId22" display="plt.subplots(figsize=(20, 10))"/>
-    <hyperlink ref="H50" location="parse_markers" display="parse_markers('punzados.txt')"/>
-    <hyperlink ref="H59" location="valores_copados" display="valores_copados"/>
-    <hyperlink ref="H68" location="get_block" display="get_block"/>
+    <hyperlink ref="H45" r:id="rId21" display="plt.subplots(figsize=(20, 10))"/>
+    <hyperlink ref="H46" r:id="rId22" display="plt.subplots(figsize=(20, 10))"/>
+    <hyperlink ref="H51" location="parse_markers" display="parse_markers('punzados.txt')"/>
+    <hyperlink ref="H60" location="valores_copados" display="valores_copados"/>
     <hyperlink ref="H69" location="get_block" display="get_block"/>
-    <hyperlink ref="H72" location="new_folder_Date" display="new_folder_date"/>
+    <hyperlink ref="H70" location="get_block" display="get_block"/>
+    <hyperlink ref="H73" location="new_folder_Date" display="new_folder_date"/>
     <hyperlink ref="H22:H23" r:id="rId23" location="collections.deque" display="collections.deque"/>
     <hyperlink ref="H24:H25" r:id="rId24" location="collections.deque" display="collections.deque"/>
     <hyperlink ref="H26" r:id="rId25" location="collections.deque"/>
     <hyperlink ref="H27:H28" r:id="rId26" location="collections.deque" display="collections.deque"/>
-    <hyperlink ref="H47" r:id="rId27"/>
-    <hyperlink ref="H48" r:id="rId28"/>
-    <hyperlink ref="H49" r:id="rId29"/>
-    <hyperlink ref="H51" r:id="rId30"/>
-    <hyperlink ref="H52" r:id="rId31"/>
-    <hyperlink ref="H55" r:id="rId32" location="matplotlib.figure.Figure.add_axes"/>
-    <hyperlink ref="H56" r:id="rId33" location="matplotlib.widgets.Slider"/>
-    <hyperlink ref="H57" r:id="rId34" location="matplotlib.figure.Figure.add_axes"/>
-    <hyperlink ref="H58" r:id="rId35" location="matplotlib.widgets.Button"/>
-    <hyperlink ref="H64" r:id="rId36" location="time.time"/>
-    <hyperlink ref="H65" r:id="rId37" location="time.time"/>
-    <hyperlink ref="H70" r:id="rId38" location="time.time"/>
-    <hyperlink ref="H71" r:id="rId39" location="time.time"/>
-    <hyperlink ref="H73" r:id="rId40" location="matplotlib-animation-funcanimation"/>
-    <hyperlink ref="H74" r:id="rId41" location="matplotlib-pyplot-plot"/>
-    <hyperlink ref="H76" location="ts_to_stringDate" display="ts_to_stringDate"/>
-    <hyperlink ref="H79" r:id="rId42" location="numpy-random-normal"/>
-    <hyperlink ref="H81" r:id="rId43"/>
-    <hyperlink ref="H83" r:id="rId44"/>
-    <hyperlink ref="H85" r:id="rId45" location="opcua.server.server.Server.register_namespace"/>
-    <hyperlink ref="H86" r:id="rId46" location="opcua.server.server.Server.get_objects_node"/>
-    <hyperlink ref="H87" r:id="rId47" location="opcua.common.node.Node.add_object"/>
-    <hyperlink ref="H89" r:id="rId48" location="opcua.common.node.Node.add_variable"/>
-    <hyperlink ref="H92" r:id="rId49" location="opcua.common.node.Node.add_variable"/>
-    <hyperlink ref="H93" r:id="rId50" location="opcua.common.node.Node.add_variable"/>
-    <hyperlink ref="H94" r:id="rId51" location="collections.deque.popleft"/>
+    <hyperlink ref="H48" r:id="rId27"/>
+    <hyperlink ref="H49" r:id="rId28"/>
+    <hyperlink ref="H50" r:id="rId29"/>
+    <hyperlink ref="H52" r:id="rId30"/>
+    <hyperlink ref="H53" r:id="rId31"/>
+    <hyperlink ref="H56" r:id="rId32" location="matplotlib.figure.Figure.add_axes"/>
+    <hyperlink ref="H57" r:id="rId33" location="matplotlib.widgets.Slider"/>
+    <hyperlink ref="H58" r:id="rId34" location="matplotlib.figure.Figure.add_axes"/>
+    <hyperlink ref="H59" r:id="rId35" location="matplotlib.widgets.Button"/>
+    <hyperlink ref="H65" r:id="rId36" location="time.time"/>
+    <hyperlink ref="H66" r:id="rId37" location="time.time"/>
+    <hyperlink ref="H71" r:id="rId38" location="time.time"/>
+    <hyperlink ref="H72" r:id="rId39" location="time.time"/>
+    <hyperlink ref="H74" r:id="rId40" location="matplotlib-animation-funcanimation"/>
+    <hyperlink ref="H75" r:id="rId41" location="matplotlib-pyplot-plot"/>
+    <hyperlink ref="H77" location="ts_to_stringDate" display="ts_to_stringDate"/>
+    <hyperlink ref="H80" r:id="rId42" location="numpy-random-normal"/>
+    <hyperlink ref="H82" r:id="rId43"/>
+    <hyperlink ref="H84" r:id="rId44"/>
+    <hyperlink ref="H86" r:id="rId45" location="opcua.server.server.Server.register_namespace"/>
+    <hyperlink ref="H87" r:id="rId46" location="opcua.server.server.Server.get_objects_node"/>
+    <hyperlink ref="H88" r:id="rId47" location="opcua.common.node.Node.add_object"/>
+    <hyperlink ref="H90" r:id="rId48" location="opcua.common.node.Node.add_variable"/>
+    <hyperlink ref="H93" r:id="rId49" location="opcua.common.node.Node.add_variable"/>
+    <hyperlink ref="H94" r:id="rId50" location="opcua.common.node.Node.add_variable"/>
+    <hyperlink ref="H95" r:id="rId51" location="collections.deque.popleft"/>
+    <hyperlink ref="D41" r:id="rId52"/>
+    <hyperlink ref="D96" r:id="rId53"/>
+    <hyperlink ref="E96" location="alarmas_queue" display="alarmas_queue"/>
+    <hyperlink ref="H97" r:id="rId54" location="glob.glob"/>
+    <hyperlink ref="H112" location="encontrar_alarmas_live" display="encontrar_alarmas_live(...)"/>
+    <hyperlink ref="H111" location="encontrar_alarmas_live" display="encontrar_alarmas_live(...)"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId52"/>
-  <legacyDrawing r:id="rId53"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId55"/>
+  <legacyDrawing r:id="rId56"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89:C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4120,7 +4913,7 @@
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4168,22 +4961,22 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="48" t="s">
         <v>247</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="48" t="s">
         <v>53</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="30"/>
+      <c r="F3" s="48"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -4191,14 +4984,14 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="30"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="48"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -4206,15 +4999,15 @@
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30" t="s">
+      <c r="A5" s="48"/>
+      <c r="B5" s="48" t="s">
         <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="33"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -4223,13 +5016,13 @@
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="33"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="51"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -4238,13 +5031,13 @@
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
+      <c r="A7" s="48"/>
+      <c r="B7" s="48"/>
       <c r="C7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="33"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -4253,19 +5046,19 @@
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="48" t="s">
         <v>81</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="51" t="s">
         <v>28</v>
       </c>
       <c r="F8" s="1"/>
@@ -4276,13 +5069,13 @@
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="48"/>
       <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="33"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="51"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -4291,13 +5084,13 @@
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="48"/>
       <c r="B10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="33"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="51"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -4306,13 +5099,13 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="48"/>
       <c r="B11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="33"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="51"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -4344,19 +5137,19 @@
       <c r="K12" s="17"/>
     </row>
     <row r="13" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="48" t="s">
         <v>85</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="51" t="s">
         <v>90</v>
       </c>
       <c r="F13" s="1"/>
@@ -4367,13 +5160,13 @@
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="48"/>
       <c r="B14" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="33"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="51"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -4382,15 +5175,15 @@
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="A15" s="48"/>
       <c r="B15" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="33"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="51"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -4399,15 +5192,15 @@
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="33"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="51"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -4416,13 +5209,13 @@
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
+      <c r="A17" s="48"/>
       <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="33"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="51"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -4494,7 +5287,7 @@
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="48" t="s">
         <v>160</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -4503,10 +5296,10 @@
       <c r="C21" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="51" t="s">
         <v>90</v>
       </c>
       <c r="F21" s="1"/>
@@ -4517,15 +5310,15 @@
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="7" t="s">
         <v>116</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D22" s="30"/>
-      <c r="E22" s="33"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="51"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
@@ -4580,17 +5373,17 @@
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="48" t="s">
         <v>163</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30" t="s">
+      <c r="C25" s="48"/>
+      <c r="D25" s="48" t="s">
         <v>179</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="51" t="s">
         <v>90</v>
       </c>
       <c r="F25" s="1"/>
@@ -4601,13 +5394,13 @@
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
+      <c r="A26" s="48"/>
       <c r="B26" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="33"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="51"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
@@ -4662,17 +5455,17 @@
       <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="48" t="s">
         <v>198</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30" t="s">
+      <c r="C29" s="48"/>
+      <c r="D29" s="48" t="s">
         <v>214</v>
       </c>
-      <c r="E29" s="33" t="s">
+      <c r="E29" s="51" t="s">
         <v>45</v>
       </c>
       <c r="F29" s="1"/>
@@ -4683,13 +5476,13 @@
       <c r="K29" s="1"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
+      <c r="A30" s="48"/>
       <c r="B30" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="33"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="51"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -4698,13 +5491,13 @@
       <c r="K30" s="1"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
+      <c r="A31" s="48"/>
       <c r="B31" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="33"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="51"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -4713,112 +5506,816 @@
       <c r="K31" s="1"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
+      <c r="A32" s="48"/>
       <c r="B32" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="33"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="51"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
+      <c r="A33" s="48"/>
       <c r="B33" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="33"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="51"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
+      <c r="A34" s="48"/>
       <c r="B34" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="33"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="51"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
+      <c r="A35" s="48"/>
       <c r="B35" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="33"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="51"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
+      <c r="A36" s="48"/>
       <c r="B36" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="33"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="51"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
+      <c r="A37" s="48"/>
       <c r="B37" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="33"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="51"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
+      <c r="A38" s="48"/>
       <c r="B38" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="33"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="51"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
+      <c r="A39" s="48"/>
       <c r="B39" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="33"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="51"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="48" t="s">
         <v>228</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="C40" s="29"/>
-      <c r="D40" s="30" t="s">
+      <c r="C40" s="54"/>
+      <c r="D40" s="48" t="s">
         <v>246</v>
       </c>
-      <c r="E40" s="28" t="s">
+      <c r="E40" s="47" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
+      <c r="A41" s="48"/>
       <c r="B41" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="C41" s="29"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="28"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="47"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
+      <c r="A42" s="48"/>
       <c r="B42" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="29"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="28"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="47"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="31" t="s">
+        <v>302</v>
+      </c>
+      <c r="C43" s="54"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="54"/>
+      <c r="B44" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="47"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="54"/>
+      <c r="B45" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="C45" s="54"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="47"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="54"/>
+      <c r="B46" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" s="54"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="47"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="54"/>
+      <c r="B47" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
+      <c r="E47" s="47"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="54"/>
+      <c r="B48" s="31" t="s">
+        <v>303</v>
+      </c>
+      <c r="C48" s="54"/>
+      <c r="D48" s="54"/>
+      <c r="E48" s="47"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="54"/>
+      <c r="B49" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" s="54"/>
+      <c r="D49" s="54"/>
+      <c r="E49" s="47"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="54"/>
+      <c r="B50" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="54"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="47"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="54"/>
+      <c r="B51" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" s="54"/>
+      <c r="D51" s="54"/>
+      <c r="E51" s="47"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="54"/>
+      <c r="B52" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="54"/>
+      <c r="D52" s="54"/>
+      <c r="E52" s="47"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="54"/>
+      <c r="B53" s="31" t="s">
+        <v>304</v>
+      </c>
+      <c r="C53" s="54"/>
+      <c r="D53" s="54"/>
+      <c r="E53" s="47"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="54"/>
+      <c r="B54" s="31" t="s">
+        <v>305</v>
+      </c>
+      <c r="C54" s="54"/>
+      <c r="D54" s="54"/>
+      <c r="E54" s="47"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="54"/>
+      <c r="B55" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C55" s="54"/>
+      <c r="D55" s="54"/>
+      <c r="E55" s="47"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="54"/>
+      <c r="B56" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="54"/>
+      <c r="D56" s="54"/>
+      <c r="E56" s="47"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="54"/>
+      <c r="B57" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57" s="54"/>
+      <c r="D57" s="54"/>
+      <c r="E57" s="47"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="54"/>
+      <c r="B58" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" s="54"/>
+      <c r="D58" s="54"/>
+      <c r="E58" s="47"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="54"/>
+      <c r="B59" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" s="54"/>
+      <c r="D59" s="54"/>
+      <c r="E59" s="47"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="54" t="s">
+        <v>337</v>
+      </c>
+      <c r="B60" s="31" t="s">
+        <v>301</v>
+      </c>
+      <c r="C60" s="54"/>
+      <c r="D60" s="54"/>
+      <c r="E60" s="47" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="54"/>
+      <c r="B61" s="31" t="s">
+        <v>302</v>
+      </c>
+      <c r="C61" s="54"/>
+      <c r="D61" s="54"/>
+      <c r="E61" s="47"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="54"/>
+      <c r="B62" s="31" t="s">
+        <v>338</v>
+      </c>
+      <c r="C62" s="54"/>
+      <c r="D62" s="54"/>
+      <c r="E62" s="47"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="54"/>
+      <c r="B63" s="31" t="s">
+        <v>339</v>
+      </c>
+      <c r="C63" s="54"/>
+      <c r="D63" s="54"/>
+      <c r="E63" s="47"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="54"/>
+      <c r="B64" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="C64" s="54"/>
+      <c r="D64" s="54"/>
+      <c r="E64" s="47"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>340</v>
+      </c>
+      <c r="B65" s="31" t="s">
+        <v>193</v>
+      </c>
+      <c r="E65" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="54" t="s">
+        <v>341</v>
+      </c>
+      <c r="B66" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="C66" s="54" t="s">
+        <v>344</v>
+      </c>
+      <c r="D66" s="54"/>
+      <c r="E66" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="54"/>
+      <c r="B67" s="31" t="s">
+        <v>343</v>
+      </c>
+      <c r="C67" s="54"/>
+      <c r="D67" s="54"/>
+      <c r="E67" s="34"/>
+    </row>
+    <row r="68" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="54" t="s">
+        <v>345</v>
+      </c>
+      <c r="B68" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="C68" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="D68" s="54"/>
+      <c r="E68" s="47" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="54"/>
+      <c r="B69" s="31" t="s">
+        <v>348</v>
+      </c>
+      <c r="C69" s="48"/>
+      <c r="D69" s="54"/>
+      <c r="E69" s="47"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="54" t="s">
+        <v>346</v>
+      </c>
+      <c r="B70" s="31" t="s">
+        <v>311</v>
+      </c>
+      <c r="C70" s="54" t="s">
+        <v>354</v>
+      </c>
+      <c r="D70" s="48" t="s">
+        <v>402</v>
+      </c>
+      <c r="E70" s="47" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="54"/>
+      <c r="B71" s="31" t="s">
+        <v>317</v>
+      </c>
+      <c r="C71" s="54"/>
+      <c r="D71" s="48"/>
+      <c r="E71" s="47"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="54"/>
+      <c r="B72" s="31" t="s">
+        <v>318</v>
+      </c>
+      <c r="C72" s="54"/>
+      <c r="D72" s="48"/>
+      <c r="E72" s="47"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="54"/>
+      <c r="B73" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C73" s="54" t="s">
+        <v>355</v>
+      </c>
+      <c r="D73" s="48"/>
+      <c r="E73" s="47"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="54"/>
+      <c r="B74" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C74" s="54"/>
+      <c r="D74" s="48"/>
+      <c r="E74" s="47"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="54"/>
+      <c r="B75" s="48" t="s">
+        <v>347</v>
+      </c>
+      <c r="C75" s="54"/>
+      <c r="D75" s="48"/>
+      <c r="E75" s="47"/>
+    </row>
+    <row r="76" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="54"/>
+      <c r="B76" s="48"/>
+      <c r="C76" s="37" t="s">
+        <v>356</v>
+      </c>
+      <c r="D76" s="48"/>
+      <c r="E76" s="47"/>
+    </row>
+    <row r="77" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="54" t="s">
+        <v>351</v>
+      </c>
+      <c r="B77" s="31" t="s">
+        <v>316</v>
+      </c>
+      <c r="C77" s="48" t="s">
+        <v>352</v>
+      </c>
+      <c r="D77" s="48" t="s">
+        <v>403</v>
+      </c>
+      <c r="E77" s="47" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="54"/>
+      <c r="B78" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C78" s="48"/>
+      <c r="D78" s="48"/>
+      <c r="E78" s="47"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="54"/>
+      <c r="B79" s="31" t="s">
+        <v>317</v>
+      </c>
+      <c r="C79" s="48"/>
+      <c r="D79" s="48"/>
+      <c r="E79" s="47"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="54"/>
+      <c r="B80" s="31" t="s">
+        <v>318</v>
+      </c>
+      <c r="C80" s="48"/>
+      <c r="D80" s="48"/>
+      <c r="E80" s="47"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="54"/>
+      <c r="B81" s="31" t="s">
+        <v>319</v>
+      </c>
+      <c r="C81" s="48"/>
+      <c r="D81" s="48"/>
+      <c r="E81" s="47"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="54"/>
+      <c r="B82" s="31" t="s">
+        <v>320</v>
+      </c>
+      <c r="C82" s="48"/>
+      <c r="D82" s="48"/>
+      <c r="E82" s="47"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="54"/>
+      <c r="B83" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C83" s="48"/>
+      <c r="D83" s="48"/>
+      <c r="E83" s="47"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="54"/>
+      <c r="B84" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="C84" s="48"/>
+      <c r="D84" s="48"/>
+      <c r="E84" s="47"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="54" t="s">
+        <v>353</v>
+      </c>
+      <c r="B85" s="31" t="s">
+        <v>328</v>
+      </c>
+      <c r="C85" t="s">
+        <v>330</v>
+      </c>
+      <c r="D85" s="54"/>
+      <c r="E85" s="47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="54"/>
+      <c r="B86" s="31" t="s">
+        <v>308</v>
+      </c>
+      <c r="C86" t="s">
+        <v>331</v>
+      </c>
+      <c r="D86" s="54"/>
+      <c r="E86" s="47"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="54"/>
+      <c r="B87" s="31" t="s">
+        <v>309</v>
+      </c>
+      <c r="C87" s="54" t="s">
+        <v>332</v>
+      </c>
+      <c r="D87" s="54"/>
+      <c r="E87" s="47"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="54"/>
+      <c r="B88" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="C88" s="54"/>
+      <c r="D88" s="54"/>
+      <c r="E88" s="47"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="54" t="s">
+        <v>389</v>
+      </c>
+      <c r="B89" s="39" t="s">
+        <v>328</v>
+      </c>
+      <c r="C89" s="54" t="s">
+        <v>325</v>
+      </c>
+      <c r="D89" s="54"/>
+      <c r="E89" s="47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="54"/>
+      <c r="B90" s="39" t="s">
+        <v>305</v>
+      </c>
+      <c r="C90" s="54"/>
+      <c r="D90" s="54"/>
+      <c r="E90" s="47"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="54"/>
+      <c r="B91" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C91" s="54"/>
+      <c r="D91" s="54"/>
+      <c r="E91" s="47"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="54"/>
+      <c r="B92" s="39" t="s">
+        <v>324</v>
+      </c>
+      <c r="C92" s="54"/>
+      <c r="D92" s="54"/>
+      <c r="E92" s="47"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="54"/>
+      <c r="B93" s="39" t="s">
+        <v>327</v>
+      </c>
+      <c r="C93" s="54"/>
+      <c r="D93" s="54"/>
+      <c r="E93" s="47"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="54"/>
+      <c r="B94" s="39" t="s">
+        <v>308</v>
+      </c>
+      <c r="C94" s="54" t="s">
+        <v>323</v>
+      </c>
+      <c r="D94" s="54"/>
+      <c r="E94" s="47"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="54"/>
+      <c r="B95" s="39" t="s">
+        <v>309</v>
+      </c>
+      <c r="C95" s="54"/>
+      <c r="D95" s="54"/>
+      <c r="E95" s="47"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="54"/>
+      <c r="B96" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="C96" s="54"/>
+      <c r="D96" s="54"/>
+      <c r="E96" s="47"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="54"/>
+      <c r="B97" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="C97" s="54"/>
+      <c r="D97" s="54"/>
+      <c r="E97" s="47"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="54"/>
+      <c r="B98" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98" s="54"/>
+      <c r="D98" s="54"/>
+      <c r="E98" s="47"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="54"/>
+      <c r="B99" s="39" t="s">
+        <v>312</v>
+      </c>
+      <c r="C99" s="54" t="s">
+        <v>324</v>
+      </c>
+      <c r="D99" s="54"/>
+      <c r="E99" s="47"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="54"/>
+      <c r="B100" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C100" s="54"/>
+      <c r="D100" s="54"/>
+      <c r="E100" s="47"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="54"/>
+      <c r="B101" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C101" s="54"/>
+      <c r="D101" s="54"/>
+      <c r="E101" s="47"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="54"/>
+      <c r="B102" s="39" t="s">
+        <v>321</v>
+      </c>
+      <c r="C102" s="54"/>
+      <c r="D102" s="54"/>
+      <c r="E102" s="47"/>
+    </row>
+    <row r="103" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="54"/>
+      <c r="B103" s="39" t="s">
+        <v>393</v>
+      </c>
+      <c r="C103" s="54"/>
+      <c r="D103" s="54"/>
+      <c r="E103" s="47"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="54"/>
+      <c r="B104" s="39" t="s">
+        <v>383</v>
+      </c>
+      <c r="C104" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="D104" s="54"/>
+      <c r="E104" s="47"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="54"/>
+      <c r="B105" s="39" t="s">
+        <v>384</v>
+      </c>
+      <c r="C105" s="54"/>
+      <c r="D105" s="54"/>
+      <c r="E105" s="47"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="54"/>
+      <c r="B106" s="39" t="s">
+        <v>325</v>
+      </c>
+      <c r="C106" s="54"/>
+      <c r="D106" s="54"/>
+      <c r="E106" s="47"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="54"/>
+      <c r="B107" s="39" t="s">
+        <v>323</v>
+      </c>
+      <c r="C107" s="54"/>
+      <c r="D107" s="54"/>
+      <c r="E107" s="47"/>
+    </row>
+    <row r="108" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="54" t="s">
+        <v>399</v>
+      </c>
+      <c r="B108" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="C108" s="54"/>
+      <c r="D108" s="48" t="s">
+        <v>401</v>
+      </c>
+      <c r="E108" s="47" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="54"/>
+      <c r="B109" s="44" t="s">
+        <v>400</v>
+      </c>
+      <c r="C109" s="54"/>
+      <c r="D109" s="48"/>
+      <c r="E109" s="47"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="70">
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="D108:D109"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="C108:C109"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="E70:E76"/>
+    <mergeCell ref="E85:E88"/>
+    <mergeCell ref="D85:D88"/>
+    <mergeCell ref="A85:A88"/>
+    <mergeCell ref="A77:A84"/>
+    <mergeCell ref="C77:C84"/>
+    <mergeCell ref="D77:D84"/>
+    <mergeCell ref="E77:E84"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="C70:C72"/>
+    <mergeCell ref="C73:C75"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="D70:D76"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="A43:A59"/>
+    <mergeCell ref="C43:C59"/>
+    <mergeCell ref="D43:D59"/>
+    <mergeCell ref="E43:E59"/>
+    <mergeCell ref="A60:A64"/>
+    <mergeCell ref="C60:C64"/>
+    <mergeCell ref="D60:D64"/>
+    <mergeCell ref="E60:E64"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="C40:C42"/>
     <mergeCell ref="D40:D42"/>
@@ -4849,6 +6346,13 @@
     <mergeCell ref="E13:E17"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A89:A107"/>
+    <mergeCell ref="D89:D107"/>
+    <mergeCell ref="E89:E107"/>
+    <mergeCell ref="C89:C93"/>
+    <mergeCell ref="C94:C98"/>
+    <mergeCell ref="C99:C103"/>
+    <mergeCell ref="C104:C107"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E13:E17" r:id="rId1" display="funciones_grafico.py"/>
@@ -4867,9 +6371,20 @@
     <hyperlink ref="E3:E7" r:id="rId14" display="func_aux_main.py"/>
     <hyperlink ref="E8:E11" r:id="rId15" display="func_aux_main.py"/>
     <hyperlink ref="E12" r:id="rId16"/>
+    <hyperlink ref="E43" r:id="rId17"/>
+    <hyperlink ref="E60" r:id="rId18" display="func_alarmas.py"/>
+    <hyperlink ref="E65" r:id="rId19"/>
+    <hyperlink ref="E66" r:id="rId20"/>
+    <hyperlink ref="E68" r:id="rId21"/>
+    <hyperlink ref="E70" r:id="rId22" display="func_alarmas.py"/>
+    <hyperlink ref="E77" r:id="rId23" display="func_alarmas.py"/>
+    <hyperlink ref="E85" r:id="rId24"/>
+    <hyperlink ref="E70:E76" r:id="rId25" display="funciones_alarmas.py"/>
+    <hyperlink ref="E60:E64" r:id="rId26" display="funciones_alarmas.py"/>
+    <hyperlink ref="E108" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId17"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId28"/>
 </worksheet>
 </file>
 

</xml_diff>